<commit_message>
Updated GridSearch Results Document
</commit_message>
<xml_diff>
--- a/JonPortion/GridSearch.xlsx
+++ b/JonPortion/GridSearch.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="973" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="Neurons in HL" sheetId="8" r:id="rId2"/>
-    <sheet name="Dropout Regularization" sheetId="7" r:id="rId3"/>
-    <sheet name="Neuron Activation Func" sheetId="6" r:id="rId4"/>
-    <sheet name="Network Weight Init" sheetId="5" r:id="rId5"/>
-    <sheet name="Learn Rate &amp; Momentum" sheetId="4" r:id="rId6"/>
-    <sheet name="Batch &amp; Epoch" sheetId="2" r:id="rId7"/>
-    <sheet name="Optimizer" sheetId="3" r:id="rId8"/>
+    <sheet name="Best" sheetId="9" r:id="rId2"/>
+    <sheet name="7. Neurons in HL" sheetId="8" r:id="rId3"/>
+    <sheet name="6. Dropout Regularization" sheetId="7" r:id="rId4"/>
+    <sheet name="5. Neuron Activation Func" sheetId="6" r:id="rId5"/>
+    <sheet name="4. Network Weight Init" sheetId="5" r:id="rId6"/>
+    <sheet name="3. Learn Rate &amp; Momentum" sheetId="4" r:id="rId7"/>
+    <sheet name="2. Optimizer" sheetId="3" r:id="rId8"/>
+    <sheet name="1. Batch &amp; Epoch" sheetId="2" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="57">
   <si>
     <t>Hyperparameter</t>
   </si>
@@ -133,6 +134,75 @@
   </si>
   <si>
     <t>neurons = [1, 5, 10, 15, 20, 25, 30]</t>
+  </si>
+  <si>
+    <t>Students</t>
+  </si>
+  <si>
+    <t>Colors</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>Weather</t>
+  </si>
+  <si>
+    <t>10/100</t>
+  </si>
+  <si>
+    <t>RMSProp</t>
+  </si>
+  <si>
+    <t>zero</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>relu</t>
+  </si>
+  <si>
+    <t>0.001/0.9</t>
+  </si>
+  <si>
+    <t>RMSprop</t>
+  </si>
+  <si>
+    <t>20/100</t>
+  </si>
+  <si>
+    <t>lecun_uniform</t>
+  </si>
+  <si>
+    <t>softplus</t>
+  </si>
+  <si>
+    <t>0.4 / 4</t>
+  </si>
+  <si>
+    <t>0.0 / 1</t>
+  </si>
+  <si>
+    <t>Batch/Epochs</t>
+  </si>
+  <si>
+    <t>Learn Rate/Momentum</t>
+  </si>
+  <si>
+    <t>0.001/0.6</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>Winner</t>
+  </si>
+  <si>
+    <t>Parameter Type</t>
   </si>
 </sst>
 </file>
@@ -192,15 +262,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>171048</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>85571</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>47223</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>142721</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -217,8 +287,84 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
+          <a:off x="485775" y="247650"/>
           <a:ext cx="3219048" cy="1228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>504457</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>114143</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="1714500"/>
+          <a:ext cx="2942857" cy="1257143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>313905</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152238</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="3238500"/>
+          <a:ext cx="3361905" cy="1295238"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -308,6 +454,158 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>485181</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>56595</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="12192000"/>
+          <a:ext cx="4752381" cy="4438095"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>589943</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>66381</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="16764000"/>
+          <a:ext cx="4857143" cy="2352381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>18438</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>94690</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="6667500"/>
+          <a:ext cx="4895238" cy="4476190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>580421</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>47344</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="628650" y="11134725"/>
+          <a:ext cx="4828571" cy="2247619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -343,6 +641,82 @@
         <a:xfrm>
           <a:off x="628650" y="200025"/>
           <a:ext cx="4047619" cy="1323810"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>580495</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>9357</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="1714500"/>
+          <a:ext cx="4238095" cy="1342857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>266209</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>142714</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="3238500"/>
+          <a:ext cx="3923809" cy="1285714"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -394,6 +768,82 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>151848</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95071</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="1714500"/>
+          <a:ext cx="4419048" cy="1428571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>190019</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>9357</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="3429000"/>
+          <a:ext cx="3847619" cy="1342857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -402,15 +852,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>104229</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>161405</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>56604</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>189980</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -427,8 +877,84 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
+          <a:off x="561975" y="219075"/>
           <a:ext cx="4371429" cy="4161905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>142324</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>18524</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="4572000"/>
+          <a:ext cx="4409524" cy="4209524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>94705</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>113786</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="9144000"/>
+          <a:ext cx="4361905" cy="4114286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -441,6 +967,125 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>85177</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>161762</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="581025" y="190500"/>
+          <a:ext cx="4380952" cy="1304762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>437713</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>28427</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="600075" y="1704975"/>
+          <a:ext cx="3495238" cy="1180952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>323352</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>190357</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="3238500"/>
+          <a:ext cx="3980952" cy="1142857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -480,41 +1125,74 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>85177</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>161762</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>466209</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>47309</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="3" name="Picture 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="581025" y="190500"/>
-          <a:ext cx="4380952" cy="1304762"/>
+          <a:off x="0" y="3810000"/>
+          <a:ext cx="4123809" cy="2523809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>494781</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>94929</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="6667500"/>
+          <a:ext cx="4152381" cy="2571429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -789,188 +1467,391 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54:C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>0.89583299999999999</v>
       </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="C6">
+        <v>0.152226</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>0.33390900000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
         <v>13</v>
       </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12">
         <v>90.833299999999994</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>0.15659799999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>0.33390900000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
         <v>16</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" t="s">
         <v>17</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C20">
         <v>0.85</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>0.144674</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>0.14825099999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
         <v>20</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D26" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C28">
         <v>0.91249999999999998</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>0.15659799999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>0.33390900000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
         <v>23</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D34" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C36">
         <v>0.91249999999999998</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>0.15659799999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>0.33390900000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
         <v>26</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D42" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
         <v>27</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D43" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C45">
         <v>0.91458300000000003</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <v>0.15143100000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>37</v>
+      </c>
+      <c r="C48" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
         <v>32</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D52" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>36</v>
+      </c>
+      <c r="C53">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C54">
         <v>0.91249999999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>35</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <v>0.15063599999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>37</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C58">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -980,29 +1861,302 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2">
+        <v>0.89583299999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>90.833299999999994</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5">
+        <v>0.91249999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6">
+        <v>0.91249999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>0.91458300000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0.91249999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9">
+        <v>0.152226</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10">
+        <v>0.15659799999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11">
+        <v>0.144674</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12">
+        <v>0.15659799999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13">
+        <v>0.15659799999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14">
+        <v>0.15143100000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0.15063599999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16">
+        <v>0.33390900000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17">
+        <v>0.33390900000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18">
+        <v>0.14825099999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19">
+        <v>0.33390900000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20">
+        <v>0.33390900000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1010,12 +2164,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A36:A74"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="K85" sqref="K85"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1023,12 +2190,30 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1036,12 +2221,30 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1049,22 +2252,27 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="K54" sqref="K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1075,12 +2283,69 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B35"/>
+  <sheetViews>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding Friendlier KerasGS Processing File
</commit_message>
<xml_diff>
--- a/JonPortion/GridSearch.xlsx
+++ b/JonPortion/GridSearch.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="973" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="973"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="58">
   <si>
     <t>Hyperparameter</t>
   </si>
@@ -203,6 +203,9 @@
   </si>
   <si>
     <t>Parameter Type</t>
+  </si>
+  <si>
+    <t>0.001 / 0.2</t>
   </si>
 </sst>
 </file>
@@ -936,11 +939,11 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>94705</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>113786</xdr:rowOff>
+      <xdr:rowOff>132833</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="5" name="Picture 4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -954,7 +957,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="609600" y="9144000"/>
-          <a:ext cx="4361905" cy="4114286"/>
+          <a:ext cx="4361905" cy="4133333"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1469,8 +1472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54:C58"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1645,12 +1648,12 @@
         <v>37</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C24">
-        <v>0.14825099999999999</v>
+        <v>0.33390900000000001</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1863,8 +1866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2054,7 +2057,7 @@
         <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D16">
         <v>0.33390900000000001</v>
@@ -2255,7 +2258,7 @@
   <dimension ref="A1:A48"/>
   <sheetViews>
     <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="K54" sqref="K54"/>
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>